<commit_message>
Apply GET and PUT method. Correct CommonRequest and CommonResponse structures.
</commit_message>
<xml_diff>
--- a/meta/objects/CommonRequest.xlsx
+++ b/meta/objects/CommonRequest.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haino/Desktop/blancoRest/meta/objects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRest/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14640" tabRatio="640"/>
   </bookViews>
   <sheets>
-    <sheet name="valueObject" sheetId="1" r:id="rId1"/>
+    <sheet name="valueObject" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Submit有無" localSheetId="0">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
+    <definedName name="Validate実装パターン" localSheetId="0">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
+    <definedName name="チェック種別" localSheetId="0">#REF!</definedName>
     <definedName name="チェック種別">#REF!</definedName>
+    <definedName name="デリミタ" localSheetId="0">#REF!</definedName>
     <definedName name="デリミタ">#REF!</definedName>
+    <definedName name="デリミタ選択肢" localSheetId="0">#REF!</definedName>
     <definedName name="デリミタ選択肢">#REF!</definedName>
+    <definedName name="型" localSheetId="0">#REF!</definedName>
     <definedName name="型">#REF!</definedName>
+    <definedName name="項目型" localSheetId="0">#REF!</definedName>
     <definedName name="項目型">#REF!</definedName>
+    <definedName name="必須" localSheetId="0">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>クラス名</t>
   </si>
@@ -61,10 +69,6 @@
   </si>
   <si>
     <t>デフォルト</t>
-  </si>
-  <si>
-    <t>様式 ver 0.0.1 (2006.11.20)</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>総称型</t>
@@ -74,100 +78,139 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>バリューオブジェクト定義書(汎用型)</t>
-    <rPh sb="14" eb="17">
-      <t>ハンヨウガ</t>
+    <t>バリューオブジェクト定義(php)・共通</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・一覧</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ApiTelegram</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>blanco.rest.valueobject</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>info</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>RequestHeader</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>通信に関するメタ情報</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>telegram</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>API毎の要求電文, ApiTelegramを継承してAPI毎に独自の型を指定</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>長さ</t>
+    <rPh sb="0" eb="1">
+      <t>ナガ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>1.このバリューオブジェクト定義書は、blancoValueObjectが入力ファイルとして利用します。</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>2.定義書様式に記入された情報から、バリューオブジェクトのための各言語ソースコードが自動生成されます。</t>
-    <rPh sb="32" eb="35">
-      <t>カクゲンゴ</t>
+    <t>値範囲Check</t>
+    <rPh sb="0" eb="1">
+      <t>アタイ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>バリューオブジェクト定義(php)・共通</t>
+    <rPh sb="1" eb="3">
+      <t>ハンイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>形式Check</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Min長</t>
+    <rPh sb="3" eb="4">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Max長</t>
+    <rPh sb="3" eb="4">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Min値</t>
+    <rPh sb="3" eb="4">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Max値</t>
+    <rPh sb="3" eb="4">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>正規表現</t>
+    <rPh sb="0" eb="2">
+      <t>セイキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヒョウゲン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義書(php)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>様式 ver 0.0.2 (2015.08.23)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1.このバリューオブジェクト定義書は、blancoValueObjectPhpが入力ファイルとして利用します。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>2.定義書様式に記入された情報から、バリューオブジェクトのためのPHPソースコードが自動生成されます。</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>名前空間</t>
+    <rPh sb="0" eb="4">
+      <t>ナマエクウカン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>blanco\rest\valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>バリューオブジェクト定義(php)・継承</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>バリューオブジェクト定義(php)・一覧</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>3.型の定義はphp様式で記述してください。</t>
-    <rPh sb="2" eb="3">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>テイギ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヨウシキ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>キジュツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>ApiTelegram</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>token</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>request</t>
+  </si>
+  <si>
+    <t>必須</t>
+  </si>
+  <si>
+    <t>共通リクエストを表すオブジェクトです。</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>CommonRequest</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>共通リクエストを表すオブジェクトです。</t>
-    <rPh sb="8" eb="9">
-      <t>アラワ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>lang</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>ja</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>認証文字列</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Apiのrequest情報</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>言語</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>blanco.rest.valueobject</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -202,7 +245,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +276,26 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -293,17 +354,6 @@
         <color indexed="8"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -548,11 +598,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -564,62 +753,90 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1029,335 +1246,608 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="5" width="23.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28" style="1" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
+    <col min="7" max="11" width="9" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="1" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="38"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+      <c r="D8" s="38"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A12" s="31" t="s">
+      <c r="C10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A13" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="48"/>
+      <c r="I16" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="48"/>
+      <c r="K16" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="49"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="9"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="14"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A18" s="18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A13" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="41" t="s">
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="14"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A19" s="18">
         <v>2</v>
       </c>
-      <c r="G16" s="41"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="19">
-        <v>1</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A19" s="19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="B19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A20" s="19">
-        <v>3</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="15"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="14"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="14"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="14"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="14"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="14"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="14"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="14"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="14"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="14"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="F16:G17"/>
+  <mergeCells count="9">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L16:M17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E41">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48 G38:K38">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>